<commit_message>
DA 18 | Day 4
</commit_message>
<xml_diff>
--- a/Batch/18/Day_3_Arithmetic.xlsx
+++ b/Batch/18/Day_3_Arithmetic.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Work\Acciojob\Modules\Excel\Batch\18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6610508B-014D-42DD-88E5-49CE32642F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1C3F07-7764-41D9-93FF-B5BBA996B30E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sum" sheetId="2" r:id="rId1"/>
     <sheet name="Sumif" sheetId="3" r:id="rId2"/>
     <sheet name="Sumifs" sheetId="4" r:id="rId3"/>
-    <sheet name="Count" sheetId="5" r:id="rId4"/>
-    <sheet name="Countif" sheetId="6" r:id="rId5"/>
-    <sheet name="Countifs" sheetId="7" r:id="rId6"/>
-    <sheet name="Average" sheetId="8" r:id="rId7"/>
-    <sheet name="Averageif" sheetId="9" r:id="rId8"/>
-    <sheet name="Averageifs" sheetId="10" r:id="rId9"/>
-    <sheet name="Sumproduct" sheetId="11" r:id="rId10"/>
+    <sheet name="Sumproduct" sheetId="11" r:id="rId4"/>
+    <sheet name="Count" sheetId="5" r:id="rId5"/>
+    <sheet name="Countif" sheetId="6" r:id="rId6"/>
+    <sheet name="Countifs" sheetId="7" r:id="rId7"/>
+    <sheet name="Average" sheetId="8" r:id="rId8"/>
+    <sheet name="Averageif" sheetId="9" r:id="rId9"/>
+    <sheet name="Averageifs" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="57">
   <si>
     <t>Sum()</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>=SUMIFS(C6:C9,C6:C9,"&gt;100",C6:C9,"&lt;500")</t>
+  </si>
+  <si>
+    <t>Array3</t>
   </si>
 </sst>
 </file>
@@ -492,17 +495,17 @@
     <xf numFmtId="165" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -577,18 +580,18 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2857500" cy="1581150"/>
+    <xdr:ext cx="2943225" cy="1647825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="image6.png">
+        <xdr:cNvPr id="2" name="image8.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -694,6 +697,45 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2857500" cy="1581150"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="image6.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>5</xdr:row>
@@ -729,7 +771,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -768,7 +810,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -807,7 +849,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -846,7 +888,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -862,45 +904,6 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2943225" cy="1647825"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="image8.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1124,7 +1127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C1:I1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
@@ -1137,14 +1140,14 @@
   <sheetData>
     <row r="1" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="25"/>
+      <c r="I2" s="26"/>
     </row>
     <row r="3" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H3" s="26"/>
-      <c r="I3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28"/>
     </row>
     <row r="4" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="5" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1180,11 +1183,11 @@
       <c r="D11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="31"/>
     </row>
     <row r="12" spans="3:9" ht="24" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C12" s="7"/>
@@ -1195,8 +1198,8 @@
       <c r="E12" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="29"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="31"/>
     </row>
     <row r="13" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C13" s="7"/>
@@ -1207,8 +1210,8 @@
       <c r="E13" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="29"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="31"/>
     </row>
     <row r="14" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="15" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2211,148 +2214,139 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="C1:I1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="B1:H1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="8.73046875" customWidth="1"/>
-    <col min="3" max="3" width="17.1328125" customWidth="1"/>
-    <col min="4" max="26" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1" width="8.73046875" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="26" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H1" s="30" t="s">
-        <v>52</v>
+    <row r="1" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G1" s="25" t="s">
+        <v>47</v>
       </c>
-      <c r="I1" s="25"/>
-    </row>
-    <row r="2" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H2" s="26"/>
-      <c r="I2" s="27"/>
-    </row>
-    <row r="3" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="5" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C5" s="35" t="s">
+      <c r="H1" s="26"/>
+    </row>
+    <row r="2" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
+    </row>
+    <row r="3" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="4" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="5" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="6" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29"/>
-    </row>
-    <row r="6" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C6" s="5">
-        <v>1</v>
+      <c r="C6" s="1"/>
+      <c r="D6" s="21"/>
+    </row>
+    <row r="7" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="14" t="s">
+        <v>25</v>
       </c>
-      <c r="D6" s="2">
-        <v>5</v>
+      <c r="C7" s="22" t="s">
+        <v>26</v>
       </c>
-      <c r="E6" s="2">
+      <c r="D7" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="23">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C7" s="5">
+      <c r="D8" s="24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="23">
+        <v>21</v>
+      </c>
+      <c r="D9" s="24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="23">
+        <v>12</v>
+      </c>
+      <c r="D10" s="24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="23">
+        <v>4</v>
+      </c>
+      <c r="D11" s="24">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="13" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="14" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="15" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="2">
-        <v>6</v>
-      </c>
-      <c r="E7" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C8" s="5">
+      <c r="C15" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="2">
-        <v>7</v>
-      </c>
-      <c r="E8" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C9" s="5">
+      <c r="D15" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="2">
-        <v>8</v>
+      <c r="E15" s="31"/>
+    </row>
+    <row r="16" spans="2:8" ht="72" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B16" s="17"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="32" t="s">
+        <v>50</v>
       </c>
-      <c r="E9" s="2">
-        <v>13</v>
+      <c r="E16" s="31"/>
+    </row>
+    <row r="17" spans="2:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B17" s="17"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="32" t="s">
+        <v>51</v>
       </c>
-    </row>
-    <row r="10" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="11" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="12" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="13" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C13" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="29"/>
-    </row>
-    <row r="14" spans="3:9" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C14" s="7"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="29"/>
-    </row>
-    <row r="15" spans="3:9" ht="36" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="29"/>
-    </row>
-    <row r="16" spans="3:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C16" s="7"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="29"/>
-    </row>
-    <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="23" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="24" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="27" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="30" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="31" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="32" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+      <c r="E17" s="31"/>
+    </row>
+    <row r="18" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="19" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="20" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="21" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="22" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="23" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="24" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="25" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="26" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="27" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="28" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="29" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="30" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="31" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="32" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -3322,13 +3316,11 @@
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="H1:I2"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="E14:I14"/>
-    <mergeCell ref="E15:I15"/>
+  <mergeCells count="4">
+    <mergeCell ref="G1:H2"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -3351,14 +3343,14 @@
   <sheetData>
     <row r="1" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="25"/>
+      <c r="I2" s="26"/>
     </row>
     <row r="3" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H3" s="26"/>
-      <c r="I3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28"/>
     </row>
     <row r="4" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="5" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -3367,7 +3359,7 @@
       <c r="C7" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="29"/>
+      <c r="D7" s="31"/>
     </row>
     <row r="8" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C8" s="5" t="s">
@@ -3410,11 +3402,11 @@
       <c r="D14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="29"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="31"/>
     </row>
     <row r="15" spans="3:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C15" s="7"/>
@@ -3422,8 +3414,8 @@
       <c r="E15" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="29"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="31"/>
     </row>
     <row r="16" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C16" s="7"/>
@@ -3431,8 +3423,8 @@
       <c r="E16" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="29"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="31"/>
     </row>
     <row r="17" spans="3:7" ht="36" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C17" s="7"/>
@@ -3440,8 +3432,8 @@
       <c r="E17" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="29"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="31"/>
     </row>
     <row r="18" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="19" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -4457,14 +4449,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="25"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="4" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -4523,10 +4515,10 @@
       <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="29"/>
+      <c r="E11" s="31"/>
     </row>
     <row r="12" spans="2:8" ht="72" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="7" t="s">
@@ -4539,7 +4531,7 @@
       <c r="D12" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="29"/>
+      <c r="E12" s="31"/>
     </row>
     <row r="13" spans="2:8" ht="67.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="7"/>
@@ -4547,7 +4539,7 @@
       <c r="D13" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="29"/>
+      <c r="E13" s="31"/>
     </row>
     <row r="14" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="7"/>
@@ -4555,7 +4547,7 @@
       <c r="D14" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="29"/>
+      <c r="E14" s="31"/>
     </row>
     <row r="15" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="16" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -5558,10 +5550,1152 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="C1:I1000"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="2" width="8.73046875" customWidth="1"/>
+    <col min="3" max="3" width="17.1328125" customWidth="1"/>
+    <col min="4" max="26" width="8.73046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="H1" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="26"/>
+    </row>
+    <row r="2" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="H2" s="27"/>
+      <c r="I2" s="28"/>
+    </row>
+    <row r="3" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="4" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="5" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C5" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="30"/>
+      <c r="E5" s="31"/>
+    </row>
+    <row r="6" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C7" s="5">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C8" s="5">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C9" s="5">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="11" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="12" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="13" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C13" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="31"/>
+    </row>
+    <row r="14" spans="3:9" ht="48" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="31"/>
+    </row>
+    <row r="15" spans="3:9" ht="36" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="31"/>
+    </row>
+    <row r="16" spans="3:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="31"/>
+    </row>
+    <row r="17" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="22" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="23" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="24" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="25" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="26" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="27" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="28" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="29" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="30" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="31" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="32" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="52" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="53" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="54" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="63" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="64" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="H1:I2"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="E15:I15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:H1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
@@ -5574,15 +6708,15 @@
   <sheetData>
     <row r="1" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B1" s="13"/>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="25"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="13"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="13"/>
@@ -8623,11 +9757,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="C1:I1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
@@ -8642,10 +9778,10 @@
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="25"/>
+      <c r="I1" s="26"/>
     </row>
     <row r="2" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C2" s="13"/>
@@ -8653,8 +9789,8 @@
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28"/>
     </row>
     <row r="3" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C3" s="13"/>
@@ -8755,11 +9891,11 @@
       <c r="D13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="29"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="31"/>
     </row>
     <row r="14" spans="3:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C14" s="17"/>
@@ -8767,8 +9903,8 @@
       <c r="E14" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="29"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="31"/>
     </row>
     <row r="15" spans="3:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C15" s="17"/>
@@ -8776,8 +9912,8 @@
       <c r="E15" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="29"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="31"/>
     </row>
     <row r="16" spans="3:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C16" s="17"/>
@@ -8785,8 +9921,8 @@
       <c r="E16" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="29"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="31"/>
     </row>
     <row r="17" spans="3:7" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C17" s="17"/>
@@ -8794,8 +9930,8 @@
       <c r="E17" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="29"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="31"/>
     </row>
     <row r="18" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C18" s="13"/>
@@ -15693,7 +16829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B1:H1000"/>
   <sheetViews>
@@ -15709,14 +16845,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="25"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="4" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -15779,11 +16915,11 @@
       <c r="C13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="29"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="31"/>
     </row>
     <row r="14" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="7"/>
@@ -15791,8 +16927,8 @@
       <c r="D14" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="28"/>
-      <c r="F14" s="29"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="31"/>
     </row>
     <row r="15" spans="2:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="7"/>
@@ -15800,8 +16936,8 @@
       <c r="D15" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31"/>
     </row>
     <row r="16" spans="2:8" ht="63" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="7"/>
@@ -15809,8 +16945,8 @@
       <c r="D16" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="28"/>
-      <c r="F16" s="29"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="31"/>
     </row>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -16810,7 +17946,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="C1:I1000"/>
   <sheetViews>
@@ -16825,14 +17961,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="25"/>
+      <c r="I1" s="26"/>
     </row>
     <row r="2" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H2" s="26"/>
-      <c r="I2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28"/>
     </row>
     <row r="3" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="4" spans="3:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -16878,8 +18014,8 @@
       <c r="E15" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="29"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="31"/>
     </row>
     <row r="16" spans="3:9" ht="24" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C16" s="17"/>
@@ -16887,8 +18023,8 @@
       <c r="E16" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="29"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="31"/>
     </row>
     <row r="17" spans="3:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C17" s="17"/>
@@ -16896,8 +18032,8 @@
       <c r="E17" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="29"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="31"/>
     </row>
     <row r="18" spans="3:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C18" s="17"/>
@@ -16905,8 +18041,8 @@
       <c r="E18" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="28"/>
-      <c r="G18" s="29"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="31"/>
     </row>
     <row r="19" spans="3:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C19" s="17"/>
@@ -16914,8 +18050,8 @@
       <c r="E19" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="28"/>
-      <c r="G19" s="29"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="31"/>
     </row>
     <row r="20" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="21" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -17913,7 +19049,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B1:H1000"/>
   <sheetViews>
@@ -17928,23 +19064,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="25"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="4" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="5" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="6" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="29"/>
+      <c r="C6" s="31"/>
     </row>
     <row r="7" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="5" t="s">
@@ -17996,11 +19132,11 @@
       <c r="C15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31"/>
     </row>
     <row r="16" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="7"/>
@@ -18008,8 +19144,8 @@
       <c r="D16" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="28"/>
-      <c r="F16" s="29"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="31"/>
     </row>
     <row r="17" spans="2:6" ht="39" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="7"/>
@@ -18017,8 +19153,8 @@
       <c r="D17" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="31"/>
     </row>
     <row r="18" spans="2:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="7"/>
@@ -18026,8 +19162,8 @@
       <c r="D18" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="28"/>
-      <c r="F18" s="29"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="31"/>
     </row>
     <row r="19" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="20" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -19024,1119 +20160,4 @@
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="B1:H1000"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="8.73046875" customWidth="1"/>
-    <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="26" width="8.73046875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G1" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="25"/>
-    </row>
-    <row r="2" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
-    </row>
-    <row r="3" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="5" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="6" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="21"/>
-    </row>
-    <row r="7" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="23">
-        <v>10</v>
-      </c>
-      <c r="D8" s="24">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="23">
-        <v>21</v>
-      </c>
-      <c r="D9" s="24">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="23">
-        <v>12</v>
-      </c>
-      <c r="D10" s="24">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="23">
-        <v>4</v>
-      </c>
-      <c r="D11" s="24">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="13" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="14" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="15" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="29"/>
-    </row>
-    <row r="16" spans="2:8" ht="72" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="17"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="29"/>
-    </row>
-    <row r="17" spans="2:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="17"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="29"/>
-    </row>
-    <row r="18" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="19" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="20" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="21" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="22" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="23" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="24" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="25" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="26" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="27" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="28" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="29" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="30" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="31" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="32" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="52" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="53" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="54" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="63" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="64" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="G1:H2"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>